<commit_message>
few more simple changes
</commit_message>
<xml_diff>
--- a/backend/ex_sheets/oo.xlsx
+++ b/backend/ex_sheets/oo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0a02c4a7808a1f27/Desktop/newStuff/Danalysis/ex_sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0a02c4a7808a1f27/Desktop/newStuff/Danalysis/backend/ex_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="16" documentId="11_6AE012AA7DA232F54B2696D39561FC6B141F84AA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{310E32D7-DB9D-46F9-8B38-8F09E4CFEF24}"/>
@@ -15,7 +15,18 @@
   <sheets>
     <sheet name="Intance Data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -12608,8 +12619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F2212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2076" workbookViewId="0">
-      <selection activeCell="D2092" sqref="D2092"/>
+    <sheetView tabSelected="1" topLeftCell="A2108" workbookViewId="0">
+      <selection activeCell="D2131" sqref="D2131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1171875" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>